<commit_message>
added results and update to connection.txt
</commit_message>
<xml_diff>
--- a/results_contrastive.xlsx
+++ b/results_contrastive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\001149822\personal\teseMECD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12BF058-450F-4072-BA65-FB19DBB98E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CD5A16-636C-432A-B115-131364D3C47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{225721F7-8DBD-4D17-B95F-7E9DEE6E05E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{225721F7-8DBD-4D17-B95F-7E9DEE6E05E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -853,6 +853,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228708</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>101641</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8220FE6-EEF8-8D7C-794C-2874D11695ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235450" y="12750800"/>
+          <a:ext cx="2101958" cy="793791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330201</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>146545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9CB257-D2B8-8A21-C2A9-CC0332AF2CF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4279901" y="12268200"/>
+          <a:ext cx="2768600" cy="400545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1155,7 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67347EDE-2342-4682-91F5-D15065DA83FD}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="95" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -1626,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605A86E5-B0B5-4366-A48F-36D8134D377A}">
   <dimension ref="C2:K66"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>